<commit_message>
feat: Add check gt order
</commit_message>
<xml_diff>
--- a/assets/labeling_data_info.xlsx
+++ b/assets/labeling_data_info.xlsx
@@ -1418,6 +1418,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1477,7 +1478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1488,6 +1489,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1510,7 +1515,7 @@
   <dimension ref="A1:AA202"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1583,14 +1588,14 @@
         <v>7</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
       <c r="R2" s="2"/>
       <c r="S2" s="1" t="s">
         <v>12</v>
@@ -1634,7 +1639,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1" t="n">
@@ -1647,23 +1652,23 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R3" s="2"/>
@@ -1695,7 +1700,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1705,32 +1710,32 @@
         <v>38</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="3"/>
       <c r="M4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="2"/>
       <c r="S4" s="1" t="s">
         <v>41</v>
@@ -1760,7 +1765,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -1770,20 +1775,20 @@
         <v>49</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="1" t="n">
@@ -1827,7 +1832,7 @@
       </c>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -1837,20 +1842,20 @@
         <v>60</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="1" t="n">
@@ -1892,7 +1897,7 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -1902,20 +1907,20 @@
         <v>68</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1" t="n">
@@ -1957,7 +1962,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1967,20 +1972,20 @@
         <v>75</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="1" t="n">
@@ -2020,7 +2025,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -2030,20 +2035,20 @@
         <v>80</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="1" t="n">
@@ -2081,7 +2086,7 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -2091,20 +2096,20 @@
         <v>84</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -2138,30 +2143,30 @@
         <v>87</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="1" t="s">
@@ -2185,36 +2190,36 @@
         <v>90</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1" t="s">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="3" t="s">
         <v>91</v>
       </c>
       <c r="R12" s="2"/>
@@ -2242,32 +2247,32 @@
         <v>94</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="1" t="s">
@@ -2281,7 +2286,7 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -2291,7 +2296,7 @@
         <v>96</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1" t="n">
@@ -2304,7 +2309,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="1" t="n">
@@ -2348,20 +2353,20 @@
         <v>102</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1" t="n">
@@ -2395,7 +2400,7 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2403,20 +2408,20 @@
         <v>108</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="1" t="n">
@@ -2450,7 +2455,7 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -2460,20 +2465,20 @@
         <v>112</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="J17" s="1" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="1" t="n">
@@ -2507,7 +2512,7 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -2517,20 +2522,20 @@
         <v>116</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I18" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="J18" s="1" t="n">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="1" t="n">
@@ -2562,7 +2567,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -2579,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>7</v>
       </c>
       <c r="J19" s="1" t="n">
         <v>84</v>
@@ -2617,7 +2622,7 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
@@ -2634,10 +2639,10 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>8</v>
       </c>
       <c r="J20" s="1" t="n">
         <v>85</v>
@@ -2691,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>1</v>
@@ -2729,7 +2734,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -2746,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>2</v>
@@ -2784,7 +2789,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -2839,7 +2844,7 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="76.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -2856,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I24" s="1" t="n">
         <v>4</v>
@@ -2894,7 +2899,7 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -2911,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>5</v>
@@ -2949,7 +2954,7 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2966,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>6</v>
@@ -3004,7 +3009,7 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
@@ -3021,7 +3026,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>7</v>
@@ -3059,7 +3064,7 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
@@ -3076,7 +3081,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I28" s="1" t="n">
         <v>8</v>
@@ -3114,7 +3119,7 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
@@ -3124,20 +3129,20 @@
         <v>162</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I29" s="1" t="n">
         <v>9</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="1" t="n">
@@ -3169,7 +3174,7 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
@@ -3179,20 +3184,20 @@
         <v>163</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I30" s="1" t="n">
         <v>10</v>
       </c>
       <c r="J30" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="1" t="n">
@@ -3224,7 +3229,7 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
@@ -3234,20 +3239,20 @@
         <v>166</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1" t="n">
         <v>11</v>
       </c>
       <c r="J31" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="1" t="n">
@@ -3279,7 +3284,7 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -3289,20 +3294,20 @@
         <v>171</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I32" s="1" t="n">
         <v>12</v>
       </c>
       <c r="J32" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="1" t="n">
@@ -3334,7 +3339,7 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
@@ -3344,20 +3349,20 @@
         <v>175</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>13</v>
       </c>
       <c r="J33" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="1" t="n">
@@ -3389,7 +3394,7 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -3399,20 +3404,20 @@
         <v>180</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>14</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="1" t="n">
@@ -3444,7 +3449,7 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
@@ -3454,20 +3459,20 @@
         <v>184</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>15</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="1" t="n">
@@ -3499,7 +3504,7 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="61.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -3509,20 +3514,20 @@
         <v>188</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>16</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="1" t="n">
@@ -3554,7 +3559,7 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="61.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
@@ -3564,20 +3569,20 @@
         <v>192</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I37" s="1" t="n">
         <v>17</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="1" t="n">
@@ -3609,7 +3614,7 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -3619,20 +3624,20 @@
         <v>195</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>18</v>
       </c>
       <c r="J38" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -3662,30 +3667,30 @@
         <v>196</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I39" s="1" t="n">
         <v>19</v>
       </c>
       <c r="J39" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K39" s="2"/>
-      <c r="L39" s="1" t="s">
+      <c r="L39" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
@@ -3707,36 +3712,36 @@
         <v>198</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I40" s="1" t="n">
         <v>20</v>
       </c>
       <c r="J40" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K40" s="2"/>
-      <c r="L40" s="1" t="s">
+      <c r="L40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="M40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1" t="s">
+      <c r="N40" s="3"/>
+      <c r="O40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="P40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="Q40" s="3" t="s">
         <v>91</v>
       </c>
       <c r="R40" s="2"/>
@@ -3750,7 +3755,7 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
@@ -3760,32 +3765,32 @@
         <v>199</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>21</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K41" s="2"/>
-      <c r="L41" s="1"/>
+      <c r="L41" s="3"/>
       <c r="M41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
@@ -3797,7 +3802,7 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
@@ -3807,20 +3812,20 @@
         <v>200</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I42" s="1" t="n">
         <v>22</v>
       </c>
       <c r="J42" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="1" t="n">
@@ -3852,7 +3857,7 @@
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
@@ -3862,20 +3867,20 @@
         <v>201</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="I43" s="1" t="n">
         <v>23</v>
       </c>
       <c r="J43" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="1" t="n">
@@ -3907,7 +3912,7 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -3917,20 +3922,20 @@
         <v>202</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="I44" s="1" t="n">
         <v>24</v>
       </c>
       <c r="J44" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="1" t="n">
@@ -3962,7 +3967,7 @@
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
@@ -3972,20 +3977,20 @@
         <v>203</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>25</v>
       </c>
       <c r="J45" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="1" t="n">
@@ -4017,7 +4022,7 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
@@ -4027,20 +4032,20 @@
         <v>204</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="I46" s="1" t="n">
         <v>26</v>
       </c>
       <c r="J46" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="1" t="n">
@@ -4072,7 +4077,7 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
@@ -4082,20 +4087,20 @@
         <v>205</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="I47" s="1" t="n">
         <v>27</v>
       </c>
       <c r="J47" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="1" t="n">
@@ -4127,7 +4132,7 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
@@ -4137,20 +4142,20 @@
         <v>206</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>28</v>
       </c>
       <c r="J48" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="1" t="n">
@@ -4182,7 +4187,7 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
@@ -4192,20 +4197,20 @@
         <v>207</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="I49" s="1" t="n">
         <v>29</v>
       </c>
       <c r="J49" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="1" t="n">
@@ -4237,7 +4242,7 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -4247,20 +4252,20 @@
         <v>208</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="I50" s="1" t="n">
         <v>30</v>
       </c>
       <c r="J50" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="1" t="n">
@@ -4292,7 +4297,7 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
@@ -4302,20 +4307,20 @@
         <v>209</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="I51" s="1" t="n">
         <v>31</v>
       </c>
       <c r="J51" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="1" t="n">
@@ -4347,7 +4352,7 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="76.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
@@ -4357,20 +4362,20 @@
         <v>210</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="I52" s="1" t="n">
         <v>32</v>
       </c>
       <c r="J52" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="1" t="n">
@@ -4402,7 +4407,7 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
@@ -4412,20 +4417,20 @@
         <v>211</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="I53" s="1" t="n">
         <v>33</v>
       </c>
       <c r="J53" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="1" t="n">
@@ -4457,7 +4462,7 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
@@ -4467,20 +4472,20 @@
         <v>212</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="I54" s="1" t="n">
         <v>34</v>
       </c>
       <c r="J54" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="1" t="n">
@@ -4512,7 +4517,7 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
@@ -4522,20 +4527,20 @@
         <v>171</v>
       </c>
       <c r="E55" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H55" s="1" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I55" s="1" t="n">
         <v>35</v>
       </c>
       <c r="J55" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="1" t="n">
@@ -4567,7 +4572,7 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -4577,20 +4582,20 @@
         <v>213</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="I56" s="1" t="n">
         <v>36</v>
       </c>
       <c r="J56" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="1" t="n">
@@ -4622,7 +4627,7 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
@@ -4632,20 +4637,20 @@
         <v>217</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="I57" s="1" t="n">
         <v>37</v>
       </c>
       <c r="J57" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="1" t="n">
@@ -4677,7 +4682,7 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -4687,20 +4692,20 @@
         <v>220</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="I58" s="1" t="n">
         <v>38</v>
       </c>
       <c r="J58" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K58" s="2"/>
       <c r="L58" s="1" t="n">
@@ -4732,7 +4737,7 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
@@ -4742,20 +4747,20 @@
         <v>221</v>
       </c>
       <c r="E59" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="I59" s="1" t="n">
         <v>39</v>
       </c>
       <c r="J59" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K59" s="2"/>
       <c r="L59" s="1" t="n">
@@ -4787,7 +4792,7 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
@@ -4797,20 +4802,20 @@
         <v>222</v>
       </c>
       <c r="E60" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="I60" s="1" t="n">
         <v>40</v>
       </c>
       <c r="J60" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K60" s="2"/>
       <c r="L60" s="1" t="n">
@@ -4842,7 +4847,7 @@
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
@@ -4852,20 +4857,20 @@
         <v>180</v>
       </c>
       <c r="E61" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I61" s="1" t="n">
         <v>41</v>
       </c>
       <c r="J61" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K61" s="2"/>
       <c r="L61" s="1" t="n">
@@ -4897,7 +4902,7 @@
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -4907,20 +4912,20 @@
         <v>223</v>
       </c>
       <c r="E62" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H62" s="1" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="I62" s="1" t="n">
         <v>42</v>
       </c>
       <c r="J62" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="1" t="n">
@@ -4952,7 +4957,7 @@
       <c r="Z62" s="2"/>
       <c r="AA62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
@@ -4962,20 +4967,20 @@
         <v>224</v>
       </c>
       <c r="E63" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H63" s="1" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="I63" s="1" t="n">
         <v>43</v>
       </c>
       <c r="J63" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K63" s="2"/>
       <c r="L63" s="1" t="n">
@@ -5007,7 +5012,7 @@
       <c r="Z63" s="2"/>
       <c r="AA63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
@@ -5017,20 +5022,20 @@
         <v>225</v>
       </c>
       <c r="E64" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="I64" s="1" t="n">
         <v>44</v>
       </c>
       <c r="J64" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K64" s="2"/>
       <c r="L64" s="1" t="n">
@@ -5062,7 +5067,7 @@
       <c r="Z64" s="2"/>
       <c r="AA64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
@@ -5072,20 +5077,20 @@
         <v>226</v>
       </c>
       <c r="E65" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H65" s="1" t="n">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="I65" s="1" t="n">
         <v>45</v>
       </c>
       <c r="J65" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K65" s="2"/>
       <c r="L65" s="1" t="n">
@@ -5129,20 +5134,20 @@
         <v>228</v>
       </c>
       <c r="E66" s="1" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I66" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J66" s="1" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K66" s="2"/>
       <c r="L66" s="1" t="n">
@@ -5174,7 +5179,7 @@
       <c r="Z66" s="2"/>
       <c r="AA66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="61.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
@@ -5191,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I67" s="1" t="n">
         <v>2</v>
@@ -5229,7 +5234,7 @@
       <c r="Z67" s="2"/>
       <c r="AA67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -5246,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I68" s="1" t="n">
         <v>3</v>
@@ -5284,7 +5289,7 @@
       <c r="Z68" s="2"/>
       <c r="AA68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
@@ -5339,7 +5344,7 @@
       <c r="Z69" s="2"/>
       <c r="AA69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="106.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="106.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
@@ -5356,7 +5361,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I70" s="1" t="n">
         <v>5</v>
@@ -5394,7 +5399,7 @@
       <c r="Z70" s="2"/>
       <c r="AA70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="76.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
@@ -5411,7 +5416,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I71" s="1" t="n">
         <v>6</v>
@@ -5461,20 +5466,20 @@
         <v>247</v>
       </c>
       <c r="E72" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I72" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J72" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="1" t="n">
@@ -5506,7 +5511,7 @@
       <c r="Z72" s="2"/>
       <c r="AA72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
@@ -5523,7 +5528,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I73" s="1" t="n">
         <v>2</v>
@@ -5561,7 +5566,7 @@
       <c r="Z73" s="2"/>
       <c r="AA73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="61.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -5578,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I74" s="1" t="n">
         <v>3</v>
@@ -5616,7 +5621,7 @@
       <c r="Z74" s="2"/>
       <c r="AA74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="46.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
@@ -5633,7 +5638,7 @@
         <v>1</v>
       </c>
       <c r="H75" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I75" s="1" t="n">
         <v>4</v>
@@ -5671,7 +5676,7 @@
       <c r="Z75" s="2"/>
       <c r="AA75" s="2"/>
     </row>
-    <row r="76" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
@@ -5726,7 +5731,7 @@
       <c r="Z76" s="2"/>
       <c r="AA76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="76.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
@@ -5743,7 +5748,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I77" s="1" t="n">
         <v>6</v>
@@ -5781,7 +5786,7 @@
       <c r="Z77" s="2"/>
       <c r="AA77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
@@ -5798,7 +5803,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I78" s="1" t="n">
         <v>7</v>
@@ -5836,7 +5841,7 @@
       <c r="Z78" s="2"/>
       <c r="AA78" s="2"/>
     </row>
-    <row r="79" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
@@ -5853,7 +5858,7 @@
         <v>1</v>
       </c>
       <c r="H79" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I79" s="1" t="n">
         <v>8</v>
@@ -5891,7 +5896,7 @@
       <c r="Z79" s="2"/>
       <c r="AA79" s="2"/>
     </row>
-    <row r="80" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
@@ -5908,7 +5913,7 @@
         <v>1</v>
       </c>
       <c r="H80" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I80" s="1" t="n">
         <v>9</v>
@@ -5946,7 +5951,7 @@
       <c r="Z80" s="2"/>
       <c r="AA80" s="2"/>
     </row>
-    <row r="81" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
@@ -5963,7 +5968,7 @@
         <v>1</v>
       </c>
       <c r="H81" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I81" s="1" t="n">
         <v>10</v>
@@ -6001,7 +6006,7 @@
       <c r="Z81" s="2"/>
       <c r="AA81" s="2"/>
     </row>
-    <row r="82" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
@@ -6018,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="H82" s="1" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I82" s="1" t="n">
         <v>11</v>
@@ -6061,7 +6066,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I83" s="1" t="n">
         <v>12</v>
@@ -6070,14 +6075,14 @@
         <v>120</v>
       </c>
       <c r="K83" s="2"/>
-      <c r="L83" s="1" t="s">
+      <c r="L83" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
-      <c r="Q83" s="1"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
       <c r="R83" s="2"/>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
@@ -6108,7 +6113,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I84" s="1" t="n">
         <v>1</v>
@@ -6117,20 +6122,20 @@
         <v>87</v>
       </c>
       <c r="K84" s="2"/>
-      <c r="L84" s="1" t="s">
+      <c r="L84" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="M84" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N84" s="1"/>
-      <c r="O84" s="1" t="s">
+      <c r="N84" s="3"/>
+      <c r="O84" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P84" s="1" t="s">
+      <c r="P84" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q84" s="1" t="s">
+      <c r="Q84" s="3" t="s">
         <v>91</v>
       </c>
       <c r="R84" s="2"/>
@@ -6144,7 +6149,7 @@
       <c r="Z84" s="2"/>
       <c r="AA84" s="2"/>
     </row>
-    <row r="85" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
@@ -6161,7 +6166,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I85" s="1" t="n">
         <v>2</v>
@@ -6170,16 +6175,16 @@
         <v>88</v>
       </c>
       <c r="K85" s="2"/>
-      <c r="L85" s="1"/>
+      <c r="L85" s="3"/>
       <c r="M85" s="1" t="s">
         <v>39</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O85" s="1"/>
-      <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
       <c r="R85" s="2"/>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
@@ -6191,7 +6196,7 @@
       <c r="Z85" s="2"/>
       <c r="AA85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
@@ -6208,7 +6213,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I86" s="1" t="n">
         <v>3</v>
@@ -6246,7 +6251,7 @@
       <c r="Z86" s="2"/>
       <c r="AA86" s="2"/>
     </row>
-    <row r="87" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
@@ -6263,7 +6268,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I87" s="1" t="n">
         <v>4</v>
@@ -6301,7 +6306,7 @@
       <c r="Z87" s="2"/>
       <c r="AA87" s="2"/>
     </row>
-    <row r="88" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
@@ -6318,7 +6323,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I88" s="1" t="n">
         <v>5</v>
@@ -6356,7 +6361,7 @@
       <c r="Z88" s="2"/>
       <c r="AA88" s="2"/>
     </row>
-    <row r="89" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
@@ -6411,7 +6416,7 @@
       <c r="Z89" s="2"/>
       <c r="AA89" s="2"/>
     </row>
-    <row r="90" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
@@ -6428,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I90" s="1" t="n">
         <v>7</v>
@@ -6466,7 +6471,7 @@
       <c r="Z90" s="2"/>
       <c r="AA90" s="2"/>
     </row>
-    <row r="91" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
@@ -6483,7 +6488,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I91" s="1" t="n">
         <v>8</v>
@@ -6538,7 +6543,7 @@
         <v>1</v>
       </c>
       <c r="H92" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I92" s="1" t="n">
         <v>9</v>
@@ -6576,7 +6581,7 @@
       <c r="Z92" s="2"/>
       <c r="AA92" s="2"/>
     </row>
-    <row r="93" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="76.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -6591,10 +6596,10 @@
         <v>1</v>
       </c>
       <c r="H93" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I93" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J93" s="1" t="n">
         <v>110</v>
@@ -6648,7 +6653,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I94" s="1" t="n">
         <v>1</v>
@@ -6686,7 +6691,7 @@
       <c r="Z94" s="2"/>
       <c r="AA94" s="2"/>
     </row>
-    <row r="95" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -6701,10 +6706,10 @@
         <v>1</v>
       </c>
       <c r="H95" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I95" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J95" s="1" t="n">
         <v>96</v>
@@ -6756,10 +6761,10 @@
         <v>1</v>
       </c>
       <c r="H96" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I96" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J96" s="1" t="n">
         <v>97</v>
@@ -6794,7 +6799,7 @@
       <c r="Z96" s="2"/>
       <c r="AA96" s="2"/>
     </row>
-    <row r="97" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -6809,10 +6814,10 @@
         <v>1</v>
       </c>
       <c r="H97" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I97" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J97" s="1" t="n">
         <v>98</v>
@@ -6847,7 +6852,7 @@
       <c r="Z97" s="2"/>
       <c r="AA97" s="2"/>
     </row>
-    <row r="98" customFormat="false" ht="121.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="121.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
@@ -6864,10 +6869,10 @@
         <v>1</v>
       </c>
       <c r="H98" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I98" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J98" s="1" t="n">
         <v>99</v>
@@ -6902,7 +6907,7 @@
       <c r="Z98" s="2"/>
       <c r="AA98" s="2"/>
     </row>
-    <row r="99" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
@@ -6919,10 +6924,10 @@
         <v>1</v>
       </c>
       <c r="H99" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I99" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J99" s="1" t="n">
         <v>100</v>
@@ -6955,7 +6960,7 @@
       <c r="Z99" s="2"/>
       <c r="AA99" s="2"/>
     </row>
-    <row r="100" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
@@ -6975,7 +6980,7 @@
         <v>7</v>
       </c>
       <c r="I100" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J100" s="1" t="n">
         <v>101</v>
@@ -7008,7 +7013,7 @@
       <c r="Z100" s="2"/>
       <c r="AA100" s="2"/>
     </row>
-    <row r="101" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
@@ -7025,10 +7030,10 @@
         <v>1</v>
       </c>
       <c r="H101" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I101" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J101" s="1" t="n">
         <v>102</v>
@@ -7063,7 +7068,7 @@
       <c r="Z101" s="2"/>
       <c r="AA101" s="2"/>
     </row>
-    <row r="102" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
@@ -7080,10 +7085,10 @@
         <v>1</v>
       </c>
       <c r="H102" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I102" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J102" s="1" t="n">
         <v>103</v>
@@ -7177,7 +7182,7 @@
       <c r="Z103" s="2"/>
       <c r="AA103" s="2"/>
     </row>
-    <row r="104" customFormat="false" ht="91.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -7195,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="I104" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J104" s="1" t="n">
         <v>135</v>
@@ -7247,10 +7252,10 @@
         <v>2</v>
       </c>
       <c r="H105" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I105" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="I105" s="1" t="n">
-        <v>3</v>
       </c>
       <c r="J105" s="1" t="n">
         <v>136</v>
@@ -7285,7 +7290,7 @@
       <c r="Z105" s="2"/>
       <c r="AA105" s="2"/>
     </row>
-    <row r="106" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -7300,10 +7305,10 @@
         <v>2</v>
       </c>
       <c r="H106" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I106" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="I106" s="1" t="n">
-        <v>4</v>
       </c>
       <c r="J106" s="1" t="n">
         <v>137</v>
@@ -7338,7 +7343,7 @@
       <c r="Z106" s="2"/>
       <c r="AA106" s="2"/>
     </row>
-    <row r="107" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -7353,10 +7358,10 @@
         <v>2</v>
       </c>
       <c r="H107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I107" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="I107" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="J107" s="1" t="n">
         <v>138</v>
@@ -7408,10 +7413,10 @@
         <v>2</v>
       </c>
       <c r="H108" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I108" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J108" s="1" t="n">
         <v>139</v>
@@ -7446,7 +7451,7 @@
       <c r="Z108" s="2"/>
       <c r="AA108" s="2"/>
     </row>
-    <row r="109" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -7461,10 +7466,10 @@
         <v>2</v>
       </c>
       <c r="H109" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I109" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J109" s="1" t="n">
         <v>140</v>
@@ -7487,7 +7492,7 @@
       <c r="Z109" s="2"/>
       <c r="AA109" s="2"/>
     </row>
-    <row r="110" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
@@ -7504,10 +7509,10 @@
         <v>2</v>
       </c>
       <c r="H110" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I110" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="I110" s="1" t="n">
-        <v>8</v>
       </c>
       <c r="J110" s="1" t="n">
         <v>141</v>
@@ -7530,7 +7535,7 @@
       <c r="Z110" s="2"/>
       <c r="AA110" s="2"/>
     </row>
-    <row r="111" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
@@ -7547,10 +7552,10 @@
         <v>2</v>
       </c>
       <c r="H111" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="I111" s="1" t="n">
-        <v>9</v>
       </c>
       <c r="J111" s="1" t="n">
         <v>142</v>
@@ -7573,7 +7578,7 @@
       <c r="Z111" s="2"/>
       <c r="AA111" s="2"/>
     </row>
-    <row r="112" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
@@ -7590,10 +7595,10 @@
         <v>2</v>
       </c>
       <c r="H112" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="I112" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="J112" s="1" t="n">
         <v>143</v>
@@ -7616,7 +7621,7 @@
       <c r="Z112" s="2"/>
       <c r="AA112" s="2"/>
     </row>
-    <row r="113" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
@@ -7633,10 +7638,10 @@
         <v>2</v>
       </c>
       <c r="H113" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="I113" s="1" t="n">
-        <v>11</v>
       </c>
       <c r="J113" s="1" t="n">
         <v>144</v>
@@ -7659,7 +7664,7 @@
       <c r="Z113" s="2"/>
       <c r="AA113" s="2"/>
     </row>
-    <row r="114" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
@@ -7676,10 +7681,10 @@
         <v>2</v>
       </c>
       <c r="H114" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" s="1" t="n">
         <v>8</v>
-      </c>
-      <c r="I114" s="1" t="n">
-        <v>12</v>
       </c>
       <c r="J114" s="1" t="n">
         <v>145</v>
@@ -7702,7 +7707,7 @@
       <c r="Z114" s="2"/>
       <c r="AA114" s="2"/>
     </row>
-    <row r="115" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
@@ -7719,10 +7724,10 @@
         <v>2</v>
       </c>
       <c r="H115" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="I115" s="1" t="n">
-        <v>13</v>
       </c>
       <c r="J115" s="1" t="n">
         <v>146</v>
@@ -7762,10 +7767,10 @@
         <v>2</v>
       </c>
       <c r="H116" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I116" s="1" t="n">
         <v>10</v>
-      </c>
-      <c r="I116" s="1" t="n">
-        <v>14</v>
       </c>
       <c r="J116" s="1" t="n">
         <v>147</v>
@@ -7788,7 +7793,7 @@
       <c r="Z116" s="2"/>
       <c r="AA116" s="2"/>
     </row>
-    <row r="117" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -7803,10 +7808,10 @@
         <v>2</v>
       </c>
       <c r="H117" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I117" s="1" t="n">
         <v>10</v>
-      </c>
-      <c r="I117" s="1" t="n">
-        <v>15</v>
       </c>
       <c r="J117" s="1" t="n">
         <v>148</v>
@@ -7841,20 +7846,20 @@
         <v>358</v>
       </c>
       <c r="E118" s="1" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H118" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I118" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J118" s="1" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
@@ -7884,7 +7889,7 @@
         <v>360</v>
       </c>
       <c r="E119" s="1" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="1" t="n">
@@ -7897,7 +7902,7 @@
         <v>2</v>
       </c>
       <c r="J119" s="1" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
@@ -7917,7 +7922,7 @@
       <c r="Z119" s="2"/>
       <c r="AA119" s="2"/>
     </row>
-    <row r="120" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -7925,7 +7930,7 @@
         <v>361</v>
       </c>
       <c r="E120" s="1" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="n">
@@ -7935,10 +7940,10 @@
         <v>2</v>
       </c>
       <c r="I120" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J120" s="1" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
@@ -7968,20 +7973,20 @@
         <v>363</v>
       </c>
       <c r="E121" s="1" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H121" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I121" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J121" s="1" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
@@ -8001,7 +8006,7 @@
       <c r="Z121" s="2"/>
       <c r="AA121" s="2"/>
     </row>
-    <row r="122" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -8009,20 +8014,20 @@
         <v>364</v>
       </c>
       <c r="E122" s="1" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F122" s="2"/>
       <c r="G122" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H122" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I122" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J122" s="1" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
@@ -8042,7 +8047,7 @@
       <c r="Z122" s="2"/>
       <c r="AA122" s="2"/>
     </row>
-    <row r="123" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1" t="s">
@@ -8052,20 +8057,20 @@
         <v>365</v>
       </c>
       <c r="E123" s="1" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H123" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I123" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I123" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="J123" s="1" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
@@ -8085,7 +8090,7 @@
       <c r="Z123" s="2"/>
       <c r="AA123" s="2"/>
     </row>
-    <row r="124" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
@@ -8095,20 +8100,20 @@
         <v>366</v>
       </c>
       <c r="E124" s="1" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H124" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I124" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I124" s="1" t="n">
-        <v>7</v>
-      </c>
       <c r="J124" s="1" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
@@ -8128,7 +8133,7 @@
       <c r="Z124" s="2"/>
       <c r="AA124" s="2"/>
     </row>
-    <row r="125" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1" t="s">
@@ -8138,20 +8143,20 @@
         <v>367</v>
       </c>
       <c r="E125" s="1" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H125" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I125" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I125" s="1" t="n">
-        <v>8</v>
-      </c>
       <c r="J125" s="1" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
@@ -8171,7 +8176,7 @@
       <c r="Z125" s="2"/>
       <c r="AA125" s="2"/>
     </row>
-    <row r="126" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
@@ -8181,20 +8186,20 @@
         <v>368</v>
       </c>
       <c r="E126" s="1" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="1" t="n">
         <v>2</v>
       </c>
       <c r="H126" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I126" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I126" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="J126" s="1" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
@@ -8214,7 +8219,7 @@
       <c r="Z126" s="2"/>
       <c r="AA126" s="2"/>
     </row>
-    <row r="127" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
@@ -8231,10 +8236,10 @@
         <v>2</v>
       </c>
       <c r="H127" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I127" s="1" t="n">
         <v>8</v>
-      </c>
-      <c r="I127" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="J127" s="1" t="n">
         <v>149</v>
@@ -8257,7 +8262,7 @@
       <c r="Z127" s="2"/>
       <c r="AA127" s="2"/>
     </row>
-    <row r="128" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
@@ -8274,10 +8279,10 @@
         <v>2</v>
       </c>
       <c r="H128" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I128" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="I128" s="1" t="n">
-        <v>11</v>
       </c>
       <c r="J128" s="1" t="n">
         <v>150</v>
@@ -8300,7 +8305,7 @@
       <c r="Z128" s="2"/>
       <c r="AA128" s="2"/>
     </row>
-    <row r="129" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
@@ -8317,10 +8322,10 @@
         <v>2</v>
       </c>
       <c r="H129" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" s="1" t="n">
         <v>10</v>
-      </c>
-      <c r="I129" s="1" t="n">
-        <v>12</v>
       </c>
       <c r="J129" s="1" t="n">
         <v>151</v>
@@ -8343,7 +8348,7 @@
       <c r="Z129" s="2"/>
       <c r="AA129" s="2"/>
     </row>
-    <row r="130" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
@@ -8360,10 +8365,10 @@
         <v>2</v>
       </c>
       <c r="H130" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I130" s="1" t="n">
         <v>11</v>
-      </c>
-      <c r="I130" s="1" t="n">
-        <v>13</v>
       </c>
       <c r="J130" s="1" t="n">
         <v>152</v>
@@ -8386,7 +8391,7 @@
       <c r="Z130" s="2"/>
       <c r="AA130" s="2"/>
     </row>
-    <row r="131" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
@@ -8403,10 +8408,10 @@
         <v>2</v>
       </c>
       <c r="H131" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I131" s="1" t="n">
         <v>12</v>
-      </c>
-      <c r="I131" s="1" t="n">
-        <v>14</v>
       </c>
       <c r="J131" s="1" t="n">
         <v>153</v>
@@ -8446,10 +8451,10 @@
         <v>2</v>
       </c>
       <c r="H132" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I132" s="1" t="n">
         <v>13</v>
-      </c>
-      <c r="I132" s="1" t="n">
-        <v>15</v>
       </c>
       <c r="J132" s="1" t="n">
         <v>154</v>
@@ -8472,7 +8477,7 @@
       <c r="Z132" s="2"/>
       <c r="AA132" s="2"/>
     </row>
-    <row r="133" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -8487,10 +8492,10 @@
         <v>2</v>
       </c>
       <c r="H133" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I133" s="1" t="n">
         <v>13</v>
-      </c>
-      <c r="I133" s="1" t="n">
-        <v>16</v>
       </c>
       <c r="J133" s="1" t="n">
         <v>155</v>
@@ -8513,7 +8518,7 @@
       <c r="Z133" s="2"/>
       <c r="AA133" s="2"/>
     </row>
-    <row r="134" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
@@ -8530,10 +8535,10 @@
         <v>2</v>
       </c>
       <c r="H134" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I134" s="1" t="n">
         <v>14</v>
-      </c>
-      <c r="I134" s="1" t="n">
-        <v>17</v>
       </c>
       <c r="J134" s="1" t="n">
         <v>156</v>
@@ -8556,7 +8561,7 @@
       <c r="Z134" s="2"/>
       <c r="AA134" s="2"/>
     </row>
-    <row r="135" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
@@ -8573,10 +8578,10 @@
         <v>2</v>
       </c>
       <c r="H135" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I135" s="1" t="n">
         <v>15</v>
-      </c>
-      <c r="I135" s="1" t="n">
-        <v>18</v>
       </c>
       <c r="J135" s="1" t="n">
         <v>157</v>
@@ -8599,7 +8604,7 @@
       <c r="Z135" s="2"/>
       <c r="AA135" s="2"/>
     </row>
-    <row r="136" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
@@ -8616,10 +8621,10 @@
         <v>2</v>
       </c>
       <c r="H136" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I136" s="1" t="n">
         <v>16</v>
-      </c>
-      <c r="I136" s="1" t="n">
-        <v>19</v>
       </c>
       <c r="J136" s="1" t="n">
         <v>158</v>
@@ -8642,7 +8647,7 @@
       <c r="Z136" s="2"/>
       <c r="AA136" s="2"/>
     </row>
-    <row r="137" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
@@ -8659,10 +8664,10 @@
         <v>2</v>
       </c>
       <c r="H137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I137" s="1" t="n">
         <v>17</v>
-      </c>
-      <c r="I137" s="1" t="n">
-        <v>20</v>
       </c>
       <c r="J137" s="1" t="n">
         <v>159</v>
@@ -8685,7 +8690,7 @@
       <c r="Z137" s="2"/>
       <c r="AA137" s="2"/>
     </row>
-    <row r="138" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
@@ -8702,10 +8707,10 @@
         <v>2</v>
       </c>
       <c r="H138" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I138" s="1" t="n">
         <v>18</v>
-      </c>
-      <c r="I138" s="1" t="n">
-        <v>21</v>
       </c>
       <c r="J138" s="1" t="n">
         <v>160</v>
@@ -8728,7 +8733,7 @@
       <c r="Z138" s="2"/>
       <c r="AA138" s="2"/>
     </row>
-    <row r="139" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
@@ -8745,10 +8750,10 @@
         <v>2</v>
       </c>
       <c r="H139" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I139" s="1" t="n">
         <v>19</v>
-      </c>
-      <c r="I139" s="1" t="n">
-        <v>22</v>
       </c>
       <c r="J139" s="1" t="n">
         <v>161</v>
@@ -8790,7 +8795,7 @@
         <v>2</v>
       </c>
       <c r="H140" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I140" s="1" t="n">
         <v>1</v>
@@ -8816,7 +8821,7 @@
       <c r="Z140" s="2"/>
       <c r="AA140" s="2"/>
     </row>
-    <row r="141" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1" t="s">
@@ -8833,7 +8838,7 @@
         <v>2</v>
       </c>
       <c r="H141" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I141" s="1" t="n">
         <v>2</v>
@@ -8859,7 +8864,7 @@
       <c r="Z141" s="2"/>
       <c r="AA141" s="2"/>
     </row>
-    <row r="142" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1" t="s">
@@ -8902,7 +8907,7 @@
       <c r="Z142" s="2"/>
       <c r="AA142" s="2"/>
     </row>
-    <row r="143" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1" t="s">
@@ -8919,7 +8924,7 @@
         <v>2</v>
       </c>
       <c r="H143" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I143" s="1" t="n">
         <v>4</v>
@@ -8945,7 +8950,7 @@
       <c r="Z143" s="2"/>
       <c r="AA143" s="2"/>
     </row>
-    <row r="144" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
@@ -8962,7 +8967,7 @@
         <v>2</v>
       </c>
       <c r="H144" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I144" s="1" t="n">
         <v>5</v>
@@ -8988,7 +8993,7 @@
       <c r="Z144" s="2"/>
       <c r="AA144" s="2"/>
     </row>
-    <row r="145" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1" t="s">
@@ -9005,7 +9010,7 @@
         <v>2</v>
       </c>
       <c r="H145" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I145" s="1" t="n">
         <v>6</v>
@@ -9031,7 +9036,7 @@
       <c r="Z145" s="2"/>
       <c r="AA145" s="2"/>
     </row>
-    <row r="146" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1" t="s">
@@ -9048,7 +9053,7 @@
         <v>2</v>
       </c>
       <c r="H146" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I146" s="1" t="n">
         <v>7</v>
@@ -9074,7 +9079,7 @@
       <c r="Z146" s="2"/>
       <c r="AA146" s="2"/>
     </row>
-    <row r="147" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
@@ -9091,7 +9096,7 @@
         <v>2</v>
       </c>
       <c r="H147" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I147" s="1" t="n">
         <v>8</v>
@@ -9117,7 +9122,7 @@
       <c r="Z147" s="2"/>
       <c r="AA147" s="2"/>
     </row>
-    <row r="148" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1" t="s">
@@ -9134,7 +9139,7 @@
         <v>2</v>
       </c>
       <c r="H148" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I148" s="1" t="n">
         <v>9</v>
@@ -9160,7 +9165,7 @@
       <c r="Z148" s="2"/>
       <c r="AA148" s="2"/>
     </row>
-    <row r="149" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1" t="s">
@@ -9177,7 +9182,7 @@
         <v>2</v>
       </c>
       <c r="H149" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I149" s="1" t="n">
         <v>10</v>
@@ -9203,7 +9208,7 @@
       <c r="Z149" s="2"/>
       <c r="AA149" s="2"/>
     </row>
-    <row r="150" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
@@ -9220,7 +9225,7 @@
         <v>2</v>
       </c>
       <c r="H150" s="1" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="I150" s="1" t="n">
         <v>11</v>
@@ -9246,7 +9251,7 @@
       <c r="Z150" s="2"/>
       <c r="AA150" s="2"/>
     </row>
-    <row r="151" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1" t="s">
@@ -9263,7 +9268,7 @@
         <v>2</v>
       </c>
       <c r="H151" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I151" s="1" t="n">
         <v>12</v>
@@ -9289,7 +9294,7 @@
       <c r="Z151" s="2"/>
       <c r="AA151" s="2"/>
     </row>
-    <row r="152" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1" t="s">
@@ -9306,7 +9311,7 @@
         <v>2</v>
       </c>
       <c r="H152" s="1" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I152" s="1" t="n">
         <v>13</v>
@@ -9346,7 +9351,7 @@
         <v>399</v>
       </c>
       <c r="E153" s="1" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F153" s="2"/>
       <c r="G153" s="1" t="n">
@@ -9359,7 +9364,7 @@
         <v>1</v>
       </c>
       <c r="J153" s="1" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K153" s="2"/>
       <c r="L153" s="2"/>
@@ -9379,7 +9384,7 @@
       <c r="Z153" s="2"/>
       <c r="AA153" s="2"/>
     </row>
-    <row r="154" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1" t="s">
@@ -9389,20 +9394,20 @@
         <v>400</v>
       </c>
       <c r="E154" s="1" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H154" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I154" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J154" s="1" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
@@ -9422,7 +9427,7 @@
       <c r="Z154" s="2"/>
       <c r="AA154" s="2"/>
     </row>
-    <row r="155" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1" t="s">
@@ -9432,20 +9437,20 @@
         <v>401</v>
       </c>
       <c r="E155" s="1" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H155" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I155" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J155" s="1" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
@@ -9465,7 +9470,7 @@
       <c r="Z155" s="2"/>
       <c r="AA155" s="2"/>
     </row>
-    <row r="156" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1" t="s">
@@ -9475,20 +9480,20 @@
         <v>402</v>
       </c>
       <c r="E156" s="1" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F156" s="2"/>
       <c r="G156" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H156" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I156" s="1" t="n">
         <v>4</v>
       </c>
       <c r="J156" s="1" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K156" s="2"/>
       <c r="L156" s="2"/>
@@ -9508,7 +9513,7 @@
       <c r="Z156" s="2"/>
       <c r="AA156" s="2"/>
     </row>
-    <row r="157" customFormat="false" ht="46.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1" t="s">
@@ -9518,20 +9523,20 @@
         <v>403</v>
       </c>
       <c r="E157" s="1" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F157" s="2"/>
       <c r="G157" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H157" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I157" s="1" t="n">
         <v>5</v>
       </c>
       <c r="J157" s="1" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
@@ -9551,7 +9556,7 @@
       <c r="Z157" s="2"/>
       <c r="AA157" s="2"/>
     </row>
-    <row r="158" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1" t="s">
@@ -9561,20 +9566,20 @@
         <v>404</v>
       </c>
       <c r="E158" s="1" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H158" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I158" s="1" t="n">
         <v>6</v>
       </c>
       <c r="J158" s="1" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
@@ -9594,7 +9599,7 @@
       <c r="Z158" s="2"/>
       <c r="AA158" s="2"/>
     </row>
-    <row r="159" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
@@ -9604,20 +9609,20 @@
         <v>405</v>
       </c>
       <c r="E159" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H159" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I159" s="1" t="n">
         <v>7</v>
       </c>
       <c r="J159" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K159" s="2"/>
       <c r="L159" s="2"/>
@@ -9637,7 +9642,7 @@
       <c r="Z159" s="2"/>
       <c r="AA159" s="2"/>
     </row>
-    <row r="160" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1" t="s">
@@ -9647,20 +9652,20 @@
         <v>406</v>
       </c>
       <c r="E160" s="1" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F160" s="2"/>
       <c r="G160" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H160" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I160" s="1" t="n">
         <v>8</v>
       </c>
       <c r="J160" s="1" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
@@ -9680,7 +9685,7 @@
       <c r="Z160" s="2"/>
       <c r="AA160" s="2"/>
     </row>
-    <row r="161" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
@@ -9690,20 +9695,20 @@
         <v>407</v>
       </c>
       <c r="E161" s="1" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F161" s="2"/>
       <c r="G161" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H161" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I161" s="1" t="n">
         <v>9</v>
       </c>
       <c r="J161" s="1" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
@@ -9723,7 +9728,7 @@
       <c r="Z161" s="2"/>
       <c r="AA161" s="2"/>
     </row>
-    <row r="162" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1" t="s">
@@ -9733,20 +9738,20 @@
         <v>408</v>
       </c>
       <c r="E162" s="1" t="n">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F162" s="2"/>
       <c r="G162" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H162" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I162" s="1" t="n">
         <v>10</v>
       </c>
       <c r="J162" s="1" t="n">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K162" s="2"/>
       <c r="L162" s="2"/>
@@ -9766,7 +9771,7 @@
       <c r="Z162" s="2"/>
       <c r="AA162" s="2"/>
     </row>
-    <row r="163" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1" t="s">
@@ -9776,20 +9781,20 @@
         <v>409</v>
       </c>
       <c r="E163" s="1" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H163" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I163" s="1" t="n">
         <v>11</v>
       </c>
       <c r="J163" s="1" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K163" s="2"/>
       <c r="L163" s="2"/>
@@ -9828,7 +9833,7 @@
         <v>3</v>
       </c>
       <c r="H164" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I164" s="1" t="n">
         <v>1</v>
@@ -9854,7 +9859,7 @@
       <c r="Z164" s="2"/>
       <c r="AA164" s="2"/>
     </row>
-    <row r="165" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1" t="s">
@@ -9897,7 +9902,7 @@
       <c r="Z165" s="2"/>
       <c r="AA165" s="2"/>
     </row>
-    <row r="166" customFormat="false" ht="46.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1" t="s">
@@ -9914,7 +9919,7 @@
         <v>3</v>
       </c>
       <c r="H166" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I166" s="1" t="n">
         <v>3</v>
@@ -9940,7 +9945,7 @@
       <c r="Z166" s="2"/>
       <c r="AA166" s="2"/>
     </row>
-    <row r="167" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1" t="s">
@@ -9957,7 +9962,7 @@
         <v>3</v>
       </c>
       <c r="H167" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I167" s="1" t="n">
         <v>4</v>
@@ -9983,7 +9988,7 @@
       <c r="Z167" s="2"/>
       <c r="AA167" s="2"/>
     </row>
-    <row r="168" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1" t="s">
@@ -10000,7 +10005,7 @@
         <v>3</v>
       </c>
       <c r="H168" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I168" s="1" t="n">
         <v>5</v>
@@ -10026,7 +10031,7 @@
       <c r="Z168" s="2"/>
       <c r="AA168" s="2"/>
     </row>
-    <row r="169" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1" t="s">
@@ -10043,7 +10048,7 @@
         <v>3</v>
       </c>
       <c r="H169" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I169" s="1" t="n">
         <v>6</v>
@@ -10069,7 +10074,7 @@
       <c r="Z169" s="2"/>
       <c r="AA169" s="2"/>
     </row>
-    <row r="170" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1" t="s">
@@ -10086,7 +10091,7 @@
         <v>3</v>
       </c>
       <c r="H170" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I170" s="1" t="n">
         <v>7</v>
@@ -10112,7 +10117,7 @@
       <c r="Z170" s="2"/>
       <c r="AA170" s="2"/>
     </row>
-    <row r="171" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1" t="s">
@@ -10129,7 +10134,7 @@
         <v>3</v>
       </c>
       <c r="H171" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I171" s="1" t="n">
         <v>8</v>
@@ -10155,7 +10160,7 @@
       <c r="Z171" s="2"/>
       <c r="AA171" s="2"/>
     </row>
-    <row r="172" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1" t="s">
@@ -10172,7 +10177,7 @@
         <v>3</v>
       </c>
       <c r="H172" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I172" s="1" t="n">
         <v>9</v>
@@ -10198,7 +10203,7 @@
       <c r="Z172" s="2"/>
       <c r="AA172" s="2"/>
     </row>
-    <row r="173" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1" t="s">
@@ -10215,7 +10220,7 @@
         <v>3</v>
       </c>
       <c r="H173" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I173" s="1" t="n">
         <v>10</v>
@@ -10260,7 +10265,7 @@
         <v>3</v>
       </c>
       <c r="H174" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I174" s="1" t="n">
         <v>1</v>
@@ -10286,7 +10291,7 @@
       <c r="Z174" s="2"/>
       <c r="AA174" s="2"/>
     </row>
-    <row r="175" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
@@ -10303,7 +10308,7 @@
         <v>3</v>
       </c>
       <c r="H175" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I175" s="1" t="n">
         <v>2</v>
@@ -10329,7 +10334,7 @@
       <c r="Z175" s="2"/>
       <c r="AA175" s="2"/>
     </row>
-    <row r="176" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="s">
@@ -10372,7 +10377,7 @@
       <c r="Z176" s="2"/>
       <c r="AA176" s="2"/>
     </row>
-    <row r="177" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1" t="s">
@@ -10389,7 +10394,7 @@
         <v>3</v>
       </c>
       <c r="H177" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I177" s="1" t="n">
         <v>4</v>
@@ -10415,7 +10420,7 @@
       <c r="Z177" s="2"/>
       <c r="AA177" s="2"/>
     </row>
-    <row r="178" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1" t="s">
@@ -10432,7 +10437,7 @@
         <v>3</v>
       </c>
       <c r="H178" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I178" s="1" t="n">
         <v>5</v>
@@ -10458,7 +10463,7 @@
       <c r="Z178" s="2"/>
       <c r="AA178" s="2"/>
     </row>
-    <row r="179" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1" t="s">
@@ -10475,7 +10480,7 @@
         <v>3</v>
       </c>
       <c r="H179" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I179" s="1" t="n">
         <v>6</v>
@@ -10501,7 +10506,7 @@
       <c r="Z179" s="2"/>
       <c r="AA179" s="2"/>
     </row>
-    <row r="180" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1" t="s">
@@ -10518,7 +10523,7 @@
         <v>3</v>
       </c>
       <c r="H180" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I180" s="1" t="n">
         <v>7</v>
@@ -10544,7 +10549,7 @@
       <c r="Z180" s="2"/>
       <c r="AA180" s="2"/>
     </row>
-    <row r="181" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1" t="s">
@@ -10561,7 +10566,7 @@
         <v>3</v>
       </c>
       <c r="H181" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I181" s="1" t="n">
         <v>8</v>
@@ -10587,7 +10592,7 @@
       <c r="Z181" s="2"/>
       <c r="AA181" s="2"/>
     </row>
-    <row r="182" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1" t="s">
@@ -10604,7 +10609,7 @@
         <v>3</v>
       </c>
       <c r="H182" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I182" s="1" t="n">
         <v>9</v>
@@ -10630,7 +10635,7 @@
       <c r="Z182" s="2"/>
       <c r="AA182" s="2"/>
     </row>
-    <row r="183" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1" t="s">
@@ -10647,7 +10652,7 @@
         <v>3</v>
       </c>
       <c r="H183" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I183" s="1" t="n">
         <v>10</v>
@@ -10692,7 +10697,7 @@
         <v>3</v>
       </c>
       <c r="H184" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I184" s="1" t="n">
         <v>1</v>
@@ -10718,7 +10723,7 @@
       <c r="Z184" s="2"/>
       <c r="AA184" s="2"/>
     </row>
-    <row r="185" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1" t="s">
@@ -10735,7 +10740,7 @@
         <v>3</v>
       </c>
       <c r="H185" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I185" s="1" t="n">
         <v>2</v>
@@ -10761,7 +10766,7 @@
       <c r="Z185" s="2"/>
       <c r="AA185" s="2"/>
     </row>
-    <row r="186" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1" t="s">
@@ -10778,7 +10783,7 @@
         <v>3</v>
       </c>
       <c r="H186" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I186" s="1" t="n">
         <v>3</v>
@@ -10804,7 +10809,7 @@
       <c r="Z186" s="2"/>
       <c r="AA186" s="2"/>
     </row>
-    <row r="187" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1" t="s">
@@ -10847,7 +10852,7 @@
       <c r="Z187" s="2"/>
       <c r="AA187" s="2"/>
     </row>
-    <row r="188" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1" t="s">
@@ -10864,7 +10869,7 @@
         <v>3</v>
       </c>
       <c r="H188" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I188" s="1" t="n">
         <v>5</v>
@@ -10890,7 +10895,7 @@
       <c r="Z188" s="2"/>
       <c r="AA188" s="2"/>
     </row>
-    <row r="189" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1" t="s">
@@ -10907,7 +10912,7 @@
         <v>3</v>
       </c>
       <c r="H189" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I189" s="1" t="n">
         <v>6</v>
@@ -10933,7 +10938,7 @@
       <c r="Z189" s="2"/>
       <c r="AA189" s="2"/>
     </row>
-    <row r="190" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1" t="s">
@@ -10950,7 +10955,7 @@
         <v>3</v>
       </c>
       <c r="H190" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I190" s="1" t="n">
         <v>7</v>
@@ -10976,7 +10981,7 @@
       <c r="Z190" s="2"/>
       <c r="AA190" s="2"/>
     </row>
-    <row r="191" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1" t="s">
@@ -10993,7 +10998,7 @@
         <v>3</v>
       </c>
       <c r="H191" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I191" s="1" t="n">
         <v>8</v>
@@ -11019,7 +11024,7 @@
       <c r="Z191" s="2"/>
       <c r="AA191" s="2"/>
     </row>
-    <row r="192" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1" t="s">
@@ -11036,7 +11041,7 @@
         <v>3</v>
       </c>
       <c r="H192" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I192" s="1" t="n">
         <v>9</v>
@@ -11081,7 +11086,7 @@
         <v>3</v>
       </c>
       <c r="H193" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I193" s="1" t="n">
         <v>1</v>
@@ -11107,7 +11112,7 @@
       <c r="Z193" s="2"/>
       <c r="AA193" s="2"/>
     </row>
-    <row r="194" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1" t="s">
@@ -11124,7 +11129,7 @@
         <v>3</v>
       </c>
       <c r="H194" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I194" s="1" t="n">
         <v>2</v>
@@ -11150,7 +11155,7 @@
       <c r="Z194" s="2"/>
       <c r="AA194" s="2"/>
     </row>
-    <row r="195" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1" t="s">
@@ -11167,7 +11172,7 @@
         <v>3</v>
       </c>
       <c r="H195" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I195" s="1" t="n">
         <v>3</v>
@@ -11193,7 +11198,7 @@
       <c r="Z195" s="2"/>
       <c r="AA195" s="2"/>
     </row>
-    <row r="196" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1" t="s">
@@ -11210,7 +11215,7 @@
         <v>3</v>
       </c>
       <c r="H196" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I196" s="1" t="n">
         <v>4</v>
@@ -11236,7 +11241,7 @@
       <c r="Z196" s="2"/>
       <c r="AA196" s="2"/>
     </row>
-    <row r="197" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1" t="s">
@@ -11279,7 +11284,7 @@
       <c r="Z197" s="2"/>
       <c r="AA197" s="2"/>
     </row>
-    <row r="198" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1" t="s">
@@ -11296,7 +11301,7 @@
         <v>3</v>
       </c>
       <c r="H198" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I198" s="1" t="n">
         <v>6</v>
@@ -11322,7 +11327,7 @@
       <c r="Z198" s="2"/>
       <c r="AA198" s="2"/>
     </row>
-    <row r="199" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1" t="s">
@@ -11339,7 +11344,7 @@
         <v>3</v>
       </c>
       <c r="H199" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I199" s="1" t="n">
         <v>7</v>
@@ -11365,7 +11370,7 @@
       <c r="Z199" s="2"/>
       <c r="AA199" s="2"/>
     </row>
-    <row r="200" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1" t="s">
@@ -11382,7 +11387,7 @@
         <v>3</v>
       </c>
       <c r="H200" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I200" s="1" t="n">
         <v>8</v>
@@ -11408,7 +11413,7 @@
       <c r="Z200" s="2"/>
       <c r="AA200" s="2"/>
     </row>
-    <row r="201" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1" t="s">
@@ -11425,7 +11430,7 @@
         <v>3</v>
       </c>
       <c r="H201" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I201" s="1" t="n">
         <v>9</v>
@@ -11451,7 +11456,7 @@
       <c r="Z201" s="2"/>
       <c r="AA201" s="2"/>
     </row>
-    <row r="202" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1" t="s">
@@ -11468,7 +11473,7 @@
         <v>3</v>
       </c>
       <c r="H202" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I202" s="1" t="n">
         <v>10</v>

</xml_diff>